<commit_message>
Update set from data objects
</commit_message>
<xml_diff>
--- a/test/files/from_data.xlsx
+++ b/test/files/from_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>OVERALL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,6 +34,22 @@
   </si>
   <si>
     <t>A5InteriorFruits_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A5InteriorFruits_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A5InteriorFruits_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A5InteriorFruits_7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A5InteriorFruits_8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -520,25 +536,33 @@
       <c r="AB1"/>
       <c r="AC1"/>
       <c r="AD1"/>
-      <c r="AE1"/>
+      <c r="AE1" t="s">
+        <v>5</v>
+      </c>
       <c r="AF1"/>
       <c r="AG1"/>
       <c r="AH1"/>
       <c r="AI1"/>
       <c r="AJ1"/>
-      <c r="AK1"/>
+      <c r="AK1" t="s">
+        <v>6</v>
+      </c>
       <c r="AL1"/>
       <c r="AM1"/>
       <c r="AN1"/>
       <c r="AO1"/>
       <c r="AP1"/>
-      <c r="AQ1"/>
+      <c r="AQ1" t="s">
+        <v>7</v>
+      </c>
       <c r="AR1"/>
       <c r="AS1"/>
       <c r="AT1"/>
       <c r="AU1"/>
       <c r="AV1"/>
-      <c r="AW1"/>
+      <c r="AW1" t="s">
+        <v>8</v>
+      </c>
       <c r="AX1"/>
       <c r="AY1"/>
       <c r="AZ1"/>
@@ -549,95 +573,139 @@
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L2"/>
       <c r="M2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="O2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="Q2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R2"/>
       <c r="S2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="T2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="U2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="V2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="W2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="X2"/>
       <c r="Y2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="Z2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AA2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB2"/>
-      <c r="AC2"/>
+        <v>12</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>14</v>
+      </c>
       <c r="AD2"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-      <c r="AI2"/>
+      <c r="AE2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>14</v>
+      </c>
       <c r="AJ2"/>
-      <c r="AK2"/>
-      <c r="AL2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
+      <c r="AK2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>14</v>
+      </c>
       <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
-      <c r="AS2"/>
-      <c r="AT2"/>
-      <c r="AU2"/>
+      <c r="AQ2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>14</v>
+      </c>
       <c r="AV2"/>
-      <c r="AW2"/>
-      <c r="AX2"/>
-      <c r="AY2"/>
-      <c r="AZ2"/>
-      <c r="BA2"/>
+      <c r="AW2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:53">
       <c r="A3"/>
@@ -754,10 +822,10 @@
     <row r="5" spans="1:53">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>3137</v>
@@ -823,32 +891,76 @@
       <c r="AA5">
         <v>650</v>
       </c>
-      <c r="AB5"/>
-      <c r="AC5"/>
+      <c r="AB5">
+        <v>1377</v>
+      </c>
+      <c r="AC5">
+        <v>1007</v>
+      </c>
       <c r="AD5"/>
-      <c r="AE5"/>
-      <c r="AF5"/>
-      <c r="AG5"/>
-      <c r="AH5"/>
-      <c r="AI5"/>
+      <c r="AE5">
+        <v>3137</v>
+      </c>
+      <c r="AF5">
+        <v>154</v>
+      </c>
+      <c r="AG5">
+        <v>974</v>
+      </c>
+      <c r="AH5">
+        <v>1349</v>
+      </c>
+      <c r="AI5">
+        <v>660</v>
+      </c>
       <c r="AJ5"/>
-      <c r="AK5"/>
-      <c r="AL5"/>
-      <c r="AM5"/>
-      <c r="AN5"/>
-      <c r="AO5"/>
+      <c r="AK5">
+        <v>3137</v>
+      </c>
+      <c r="AL5">
+        <v>104</v>
+      </c>
+      <c r="AM5">
+        <v>1023</v>
+      </c>
+      <c r="AN5">
+        <v>1424</v>
+      </c>
+      <c r="AO5">
+        <v>586</v>
+      </c>
       <c r="AP5"/>
-      <c r="AQ5"/>
-      <c r="AR5"/>
-      <c r="AS5"/>
-      <c r="AT5"/>
-      <c r="AU5"/>
+      <c r="AQ5">
+        <v>3137</v>
+      </c>
+      <c r="AR5">
+        <v>359</v>
+      </c>
+      <c r="AS5">
+        <v>1606</v>
+      </c>
+      <c r="AT5">
+        <v>972</v>
+      </c>
+      <c r="AU5">
+        <v>200</v>
+      </c>
       <c r="AV5"/>
-      <c r="AW5"/>
-      <c r="AX5"/>
-      <c r="AY5"/>
-      <c r="AZ5"/>
-      <c r="BA5"/>
+      <c r="AW5">
+        <v>3137</v>
+      </c>
+      <c r="AX5">
+        <v>512</v>
+      </c>
+      <c r="AY5">
+        <v>1728</v>
+      </c>
+      <c r="AZ5">
+        <v>744</v>
+      </c>
+      <c r="BA5">
+        <v>153</v>
+      </c>
     </row>
     <row r="6" spans="1:53">
       <c r="A6"/>
@@ -907,7 +1019,7 @@
     </row>
     <row r="7" spans="1:53">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7"/>
       <c r="C7"/>
@@ -965,10 +1077,10 @@
     <row r="8" spans="1:53">
       <c r="A8"/>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>0.5259802358941664</v>
@@ -1034,40 +1146,84 @@
       <c r="AA8">
         <v>0.5030769230769231</v>
       </c>
-      <c r="AB8"/>
-      <c r="AC8"/>
+      <c r="AB8">
+        <v>0.5453885257806826</v>
+      </c>
+      <c r="AC8">
+        <v>0.5163853028798411</v>
+      </c>
       <c r="AD8"/>
-      <c r="AE8"/>
-      <c r="AF8"/>
-      <c r="AG8"/>
-      <c r="AH8"/>
-      <c r="AI8"/>
+      <c r="AE8">
+        <v>0.5259802358941664</v>
+      </c>
+      <c r="AF8">
+        <v>0.487012987012987</v>
+      </c>
+      <c r="AG8">
+        <v>0.5143737166324436</v>
+      </c>
+      <c r="AH8">
+        <v>0.5174203113417346</v>
+      </c>
+      <c r="AI8">
+        <v>0.5696969696969697</v>
+      </c>
       <c r="AJ8"/>
-      <c r="AK8"/>
-      <c r="AL8"/>
-      <c r="AM8"/>
-      <c r="AN8"/>
-      <c r="AO8"/>
+      <c r="AK8">
+        <v>0.5259802358941664</v>
+      </c>
+      <c r="AL8">
+        <v>0.4423076923076923</v>
+      </c>
+      <c r="AM8">
+        <v>0.5083088954056696</v>
+      </c>
+      <c r="AN8">
+        <v>0.5428370786516854</v>
+      </c>
+      <c r="AO8">
+        <v>0.5307167235494881</v>
+      </c>
       <c r="AP8"/>
-      <c r="AQ8"/>
-      <c r="AR8"/>
-      <c r="AS8"/>
-      <c r="AT8"/>
-      <c r="AU8"/>
+      <c r="AQ8">
+        <v>0.5259802358941664</v>
+      </c>
+      <c r="AR8">
+        <v>0.46518105849582175</v>
+      </c>
+      <c r="AS8">
+        <v>0.5236612702366127</v>
+      </c>
+      <c r="AT8">
+        <v>0.5473251028806584</v>
+      </c>
+      <c r="AU8">
+        <v>0.55</v>
+      </c>
       <c r="AV8"/>
-      <c r="AW8"/>
-      <c r="AX8"/>
-      <c r="AY8"/>
-      <c r="AZ8"/>
-      <c r="BA8"/>
+      <c r="AW8">
+        <v>0.5259802358941664</v>
+      </c>
+      <c r="AX8">
+        <v>0.529296875</v>
+      </c>
+      <c r="AY8">
+        <v>0.5353009259259259</v>
+      </c>
+      <c r="AZ8">
+        <v>0.5174731182795699</v>
+      </c>
+      <c r="BA8">
+        <v>0.45098039215686275</v>
+      </c>
     </row>
     <row r="9" spans="1:53">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>0.503984698756774</v>
@@ -1133,40 +1289,84 @@
       <c r="AA9">
         <v>0.5169230769230769</v>
       </c>
-      <c r="AB9"/>
-      <c r="AC9"/>
+      <c r="AB9">
+        <v>0.49963689179375453</v>
+      </c>
+      <c r="AC9">
+        <v>0.5114200595829196</v>
+      </c>
       <c r="AD9"/>
-      <c r="AE9"/>
-      <c r="AF9"/>
-      <c r="AG9"/>
-      <c r="AH9"/>
-      <c r="AI9"/>
+      <c r="AE9">
+        <v>0.503984698756774</v>
+      </c>
+      <c r="AF9">
+        <v>0.44155844155844154</v>
+      </c>
+      <c r="AG9">
+        <v>0.48254620123203285</v>
+      </c>
+      <c r="AH9">
+        <v>0.5233506300963677</v>
+      </c>
+      <c r="AI9">
+        <v>0.5106060606060606</v>
+      </c>
       <c r="AJ9"/>
-      <c r="AK9"/>
-      <c r="AL9"/>
-      <c r="AM9"/>
-      <c r="AN9"/>
-      <c r="AO9"/>
+      <c r="AK9">
+        <v>0.503984698756774</v>
+      </c>
+      <c r="AL9">
+        <v>0.47115384615384615</v>
+      </c>
+      <c r="AM9">
+        <v>0.4965786901270772</v>
+      </c>
+      <c r="AN9">
+        <v>0.5168539325842697</v>
+      </c>
+      <c r="AO9">
+        <v>0.49146757679180886</v>
+      </c>
       <c r="AP9"/>
-      <c r="AQ9"/>
-      <c r="AR9"/>
-      <c r="AS9"/>
-      <c r="AT9"/>
-      <c r="AU9"/>
+      <c r="AQ9">
+        <v>0.503984698756774</v>
+      </c>
+      <c r="AR9">
+        <v>0.467966573816156</v>
+      </c>
+      <c r="AS9">
+        <v>0.5049813200498132</v>
+      </c>
+      <c r="AT9">
+        <v>0.5246913580246914</v>
+      </c>
+      <c r="AU9">
+        <v>0.46</v>
+      </c>
       <c r="AV9"/>
-      <c r="AW9"/>
-      <c r="AX9"/>
-      <c r="AY9"/>
-      <c r="AZ9"/>
-      <c r="BA9"/>
+      <c r="AW9">
+        <v>0.503984698756774</v>
+      </c>
+      <c r="AX9">
+        <v>0.4609375</v>
+      </c>
+      <c r="AY9">
+        <v>0.5266203703703703</v>
+      </c>
+      <c r="AZ9">
+        <v>0.4959677419354839</v>
+      </c>
+      <c r="BA9">
+        <v>0.43137254901960786</v>
+      </c>
     </row>
     <row r="10" spans="1:53">
       <c r="A10"/>
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
       </c>
       <c r="D10">
         <v>0.448836467963022</v>
@@ -1232,40 +1432,84 @@
       <c r="AA10">
         <v>0.43846153846153846</v>
       </c>
-      <c r="AB10"/>
-      <c r="AC10"/>
+      <c r="AB10">
+        <v>0.4466230936819172</v>
+      </c>
+      <c r="AC10">
+        <v>0.46772591857000995</v>
+      </c>
       <c r="AD10"/>
-      <c r="AE10"/>
-      <c r="AF10"/>
-      <c r="AG10"/>
-      <c r="AH10"/>
-      <c r="AI10"/>
+      <c r="AE10">
+        <v>0.448836467963022</v>
+      </c>
+      <c r="AF10">
+        <v>0.461038961038961</v>
+      </c>
+      <c r="AG10">
+        <v>0.41786447638603696</v>
+      </c>
+      <c r="AH10">
+        <v>0.469236471460341</v>
+      </c>
+      <c r="AI10">
+        <v>0.45</v>
+      </c>
       <c r="AJ10"/>
-      <c r="AK10"/>
-      <c r="AL10"/>
-      <c r="AM10"/>
-      <c r="AN10"/>
-      <c r="AO10"/>
+      <c r="AK10">
+        <v>0.448836467963022</v>
+      </c>
+      <c r="AL10">
+        <v>0.4423076923076923</v>
+      </c>
+      <c r="AM10">
+        <v>0.4095796676441838</v>
+      </c>
+      <c r="AN10">
+        <v>0.46769662921348315</v>
+      </c>
+      <c r="AO10">
+        <v>0.4726962457337884</v>
+      </c>
       <c r="AP10"/>
-      <c r="AQ10"/>
-      <c r="AR10"/>
-      <c r="AS10"/>
-      <c r="AT10"/>
-      <c r="AU10"/>
+      <c r="AQ10">
+        <v>0.448836467963022</v>
+      </c>
+      <c r="AR10">
+        <v>0.45125348189415043</v>
+      </c>
+      <c r="AS10">
+        <v>0.4302615193026152</v>
+      </c>
+      <c r="AT10">
+        <v>0.47016460905349794</v>
+      </c>
+      <c r="AU10">
+        <v>0.49</v>
+      </c>
       <c r="AV10"/>
-      <c r="AW10"/>
-      <c r="AX10"/>
-      <c r="AY10"/>
-      <c r="AZ10"/>
-      <c r="BA10"/>
+      <c r="AW10">
+        <v>0.448836467963022</v>
+      </c>
+      <c r="AX10">
+        <v>0.42578125</v>
+      </c>
+      <c r="AY10">
+        <v>0.4519675925925926</v>
+      </c>
+      <c r="AZ10">
+        <v>0.45564516129032256</v>
+      </c>
+      <c r="BA10">
+        <v>0.45751633986928103</v>
+      </c>
     </row>
     <row r="11" spans="1:53">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>0.1858463500159388</v>
@@ -1331,40 +1575,84 @@
       <c r="AA11">
         <v>0.20923076923076922</v>
       </c>
-      <c r="AB11"/>
-      <c r="AC11"/>
+      <c r="AB11">
+        <v>0.1924473493100944</v>
+      </c>
+      <c r="AC11">
+        <v>0.16881827209533268</v>
+      </c>
       <c r="AD11"/>
-      <c r="AE11"/>
-      <c r="AF11"/>
-      <c r="AG11"/>
-      <c r="AH11"/>
-      <c r="AI11"/>
+      <c r="AE11">
+        <v>0.1858463500159388</v>
+      </c>
+      <c r="AF11">
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="AG11">
+        <v>0.19815195071868583</v>
+      </c>
+      <c r="AH11">
+        <v>0.16604892512972572</v>
+      </c>
+      <c r="AI11">
+        <v>0.2015151515151515</v>
+      </c>
       <c r="AJ11"/>
-      <c r="AK11"/>
-      <c r="AL11"/>
-      <c r="AM11"/>
-      <c r="AN11"/>
-      <c r="AO11"/>
+      <c r="AK11">
+        <v>0.1858463500159388</v>
+      </c>
+      <c r="AL11">
+        <v>0.17307692307692307</v>
+      </c>
+      <c r="AM11">
+        <v>0.18377321603128055</v>
+      </c>
+      <c r="AN11">
+        <v>0.19803370786516855</v>
+      </c>
+      <c r="AO11">
+        <v>0.1621160409556314</v>
+      </c>
       <c r="AP11"/>
-      <c r="AQ11"/>
-      <c r="AR11"/>
-      <c r="AS11"/>
-      <c r="AT11"/>
-      <c r="AU11"/>
+      <c r="AQ11">
+        <v>0.1858463500159388</v>
+      </c>
+      <c r="AR11">
+        <v>0.1977715877437326</v>
+      </c>
+      <c r="AS11">
+        <v>0.17496886674968867</v>
+      </c>
+      <c r="AT11">
+        <v>0.20164609053497942</v>
+      </c>
+      <c r="AU11">
+        <v>0.175</v>
+      </c>
       <c r="AV11"/>
-      <c r="AW11"/>
-      <c r="AX11"/>
-      <c r="AY11"/>
-      <c r="AZ11"/>
-      <c r="BA11"/>
+      <c r="AW11">
+        <v>0.1858463500159388</v>
+      </c>
+      <c r="AX11">
+        <v>0.1796875</v>
+      </c>
+      <c r="AY11">
+        <v>0.1892361111111111</v>
+      </c>
+      <c r="AZ11">
+        <v>0.1935483870967742</v>
+      </c>
+      <c r="BA11">
+        <v>0.13071895424836602</v>
+      </c>
     </row>
     <row r="12" spans="1:53">
       <c r="A12"/>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>0.3736053554351291</v>
@@ -1430,40 +1718,84 @@
       <c r="AA12">
         <v>0.37538461538461537</v>
       </c>
-      <c r="AB12"/>
-      <c r="AC12"/>
+      <c r="AB12">
+        <v>0.3769063180827887</v>
+      </c>
+      <c r="AC12">
+        <v>0.3743793445878848</v>
+      </c>
       <c r="AD12"/>
-      <c r="AE12"/>
-      <c r="AF12"/>
-      <c r="AG12"/>
-      <c r="AH12"/>
-      <c r="AI12"/>
+      <c r="AE12">
+        <v>0.3736053554351291</v>
+      </c>
+      <c r="AF12">
+        <v>0.33766233766233766</v>
+      </c>
+      <c r="AG12">
+        <v>0.39117043121149897</v>
+      </c>
+      <c r="AH12">
+        <v>0.36619718309859156</v>
+      </c>
+      <c r="AI12">
+        <v>0.3712121212121212</v>
+      </c>
       <c r="AJ12"/>
-      <c r="AK12"/>
-      <c r="AL12"/>
-      <c r="AM12"/>
-      <c r="AN12"/>
-      <c r="AO12"/>
+      <c r="AK12">
+        <v>0.3736053554351291</v>
+      </c>
+      <c r="AL12">
+        <v>0.3557692307692308</v>
+      </c>
+      <c r="AM12">
+        <v>0.3782991202346041</v>
+      </c>
+      <c r="AN12">
+        <v>0.3714887640449438</v>
+      </c>
+      <c r="AO12">
+        <v>0.37372013651877134</v>
+      </c>
       <c r="AP12"/>
-      <c r="AQ12"/>
-      <c r="AR12"/>
-      <c r="AS12"/>
-      <c r="AT12"/>
-      <c r="AU12"/>
+      <c r="AQ12">
+        <v>0.3736053554351291</v>
+      </c>
+      <c r="AR12">
+        <v>0.3342618384401114</v>
+      </c>
+      <c r="AS12">
+        <v>0.3823163138231631</v>
+      </c>
+      <c r="AT12">
+        <v>0.39094650205761317</v>
+      </c>
+      <c r="AU12">
+        <v>0.29</v>
+      </c>
       <c r="AV12"/>
-      <c r="AW12"/>
-      <c r="AX12"/>
-      <c r="AY12"/>
-      <c r="AZ12"/>
-      <c r="BA12"/>
+      <c r="AW12">
+        <v>0.3736053554351291</v>
+      </c>
+      <c r="AX12">
+        <v>0.369140625</v>
+      </c>
+      <c r="AY12">
+        <v>0.38425925925925924</v>
+      </c>
+      <c r="AZ12">
+        <v>0.35618279569892475</v>
+      </c>
+      <c r="BA12">
+        <v>0.35294117647058826</v>
+      </c>
     </row>
     <row r="13" spans="1:53">
       <c r="A13"/>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>0.15301243226012112</v>
@@ -1529,40 +1861,84 @@
       <c r="AA13">
         <v>0.15384615384615385</v>
       </c>
-      <c r="AB13"/>
-      <c r="AC13"/>
+      <c r="AB13">
+        <v>0.14960058097313</v>
+      </c>
+      <c r="AC13">
+        <v>0.1628599801390268</v>
+      </c>
       <c r="AD13"/>
-      <c r="AE13"/>
-      <c r="AF13"/>
-      <c r="AG13"/>
-      <c r="AH13"/>
-      <c r="AI13"/>
+      <c r="AE13">
+        <v>0.15301243226012112</v>
+      </c>
+      <c r="AF13">
+        <v>0.11038961038961038</v>
+      </c>
+      <c r="AG13">
+        <v>0.14784394250513347</v>
+      </c>
+      <c r="AH13">
+        <v>0.15048183839881393</v>
+      </c>
+      <c r="AI13">
+        <v>0.17575757575757575</v>
+      </c>
       <c r="AJ13"/>
-      <c r="AK13"/>
-      <c r="AL13"/>
-      <c r="AM13"/>
-      <c r="AN13"/>
-      <c r="AO13"/>
+      <c r="AK13">
+        <v>0.15301243226012112</v>
+      </c>
+      <c r="AL13">
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="AM13">
+        <v>0.14271749755620725</v>
+      </c>
+      <c r="AN13">
+        <v>0.15098314606741572</v>
+      </c>
+      <c r="AO13">
+        <v>0.1757679180887372</v>
+      </c>
       <c r="AP13"/>
-      <c r="AQ13"/>
-      <c r="AR13"/>
-      <c r="AS13"/>
-      <c r="AT13"/>
-      <c r="AU13"/>
+      <c r="AQ13">
+        <v>0.15301243226012112</v>
+      </c>
+      <c r="AR13">
+        <v>0.12813370473537605</v>
+      </c>
+      <c r="AS13">
+        <v>0.14881693648816938</v>
+      </c>
+      <c r="AT13">
+        <v>0.16049382716049382</v>
+      </c>
+      <c r="AU13">
+        <v>0.195</v>
+      </c>
       <c r="AV13"/>
-      <c r="AW13"/>
-      <c r="AX13"/>
-      <c r="AY13"/>
-      <c r="AZ13"/>
-      <c r="BA13"/>
+      <c r="AW13">
+        <v>0.15301243226012112</v>
+      </c>
+      <c r="AX13">
+        <v>0.138671875</v>
+      </c>
+      <c r="AY13">
+        <v>0.15046296296296297</v>
+      </c>
+      <c r="AZ13">
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="BA13">
+        <v>0.1895424836601307</v>
+      </c>
     </row>
     <row r="14" spans="1:53">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>0.5890978642014664</v>
@@ -1628,40 +2004,84 @@
       <c r="AA14">
         <v>0.6030769230769231</v>
       </c>
-      <c r="AB14"/>
-      <c r="AC14"/>
+      <c r="AB14">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="AC14">
+        <v>0.5888778550148958</v>
+      </c>
       <c r="AD14"/>
-      <c r="AE14"/>
-      <c r="AF14"/>
-      <c r="AG14"/>
-      <c r="AH14"/>
-      <c r="AI14"/>
+      <c r="AE14">
+        <v>0.5890978642014664</v>
+      </c>
+      <c r="AF14">
+        <v>0.6233766233766234</v>
+      </c>
+      <c r="AG14">
+        <v>0.6149897330595483</v>
+      </c>
+      <c r="AH14">
+        <v>0.5774647887323944</v>
+      </c>
+      <c r="AI14">
+        <v>0.5666666666666667</v>
+      </c>
       <c r="AJ14"/>
-      <c r="AK14"/>
-      <c r="AL14"/>
-      <c r="AM14"/>
-      <c r="AN14"/>
-      <c r="AO14"/>
+      <c r="AK14">
+        <v>0.5890978642014664</v>
+      </c>
+      <c r="AL14">
+        <v>0.5673076923076923</v>
+      </c>
+      <c r="AM14">
+        <v>0.5806451612903226</v>
+      </c>
+      <c r="AN14">
+        <v>0.5990168539325843</v>
+      </c>
+      <c r="AO14">
+        <v>0.5836177474402731</v>
+      </c>
       <c r="AP14"/>
-      <c r="AQ14"/>
-      <c r="AR14"/>
-      <c r="AS14"/>
-      <c r="AT14"/>
-      <c r="AU14"/>
+      <c r="AQ14">
+        <v>0.5890978642014664</v>
+      </c>
+      <c r="AR14">
+        <v>0.6239554317548747</v>
+      </c>
+      <c r="AS14">
+        <v>0.5815691158156912</v>
+      </c>
+      <c r="AT14">
+        <v>0.5997942386831275</v>
+      </c>
+      <c r="AU14">
+        <v>0.535</v>
+      </c>
       <c r="AV14"/>
-      <c r="AW14"/>
-      <c r="AX14"/>
-      <c r="AY14"/>
-      <c r="AZ14"/>
-      <c r="BA14"/>
+      <c r="AW14">
+        <v>0.5890978642014664</v>
+      </c>
+      <c r="AX14">
+        <v>0.62890625</v>
+      </c>
+      <c r="AY14">
+        <v>0.5983796296296297</v>
+      </c>
+      <c r="AZ14">
+        <v>0.5524193548387096</v>
+      </c>
+      <c r="BA14">
+        <v>0.5294117647058824</v>
+      </c>
     </row>
     <row r="15" spans="1:53">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <v>0.8138348740835193</v>
@@ -1727,40 +2147,84 @@
       <c r="AA15">
         <v>0.8215384615384616</v>
       </c>
-      <c r="AB15"/>
-      <c r="AC15"/>
+      <c r="AB15">
+        <v>0.8126361655773421</v>
+      </c>
+      <c r="AC15">
+        <v>0.8073485600794439</v>
+      </c>
       <c r="AD15"/>
-      <c r="AE15"/>
-      <c r="AF15"/>
-      <c r="AG15"/>
-      <c r="AH15"/>
-      <c r="AI15"/>
+      <c r="AE15">
+        <v>0.8138348740835193</v>
+      </c>
+      <c r="AF15">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="AG15">
+        <v>0.797741273100616</v>
+      </c>
+      <c r="AH15">
+        <v>0.816160118606375</v>
+      </c>
+      <c r="AI15">
+        <v>0.8393939393939394</v>
+      </c>
       <c r="AJ15"/>
-      <c r="AK15"/>
-      <c r="AL15"/>
-      <c r="AM15"/>
-      <c r="AN15"/>
-      <c r="AO15"/>
+      <c r="AK15">
+        <v>0.8138348740835193</v>
+      </c>
+      <c r="AL15">
+        <v>0.7692307692307693</v>
+      </c>
+      <c r="AM15">
+        <v>0.8103616813294232</v>
+      </c>
+      <c r="AN15">
+        <v>0.8230337078651685</v>
+      </c>
+      <c r="AO15">
+        <v>0.8054607508532423</v>
+      </c>
       <c r="AP15"/>
-      <c r="AQ15"/>
-      <c r="AR15"/>
-      <c r="AS15"/>
-      <c r="AT15"/>
-      <c r="AU15"/>
+      <c r="AQ15">
+        <v>0.8138348740835193</v>
+      </c>
+      <c r="AR15">
+        <v>0.7910863509749304</v>
+      </c>
+      <c r="AS15">
+        <v>0.811332503113325</v>
+      </c>
+      <c r="AT15">
+        <v>0.8261316872427984</v>
+      </c>
+      <c r="AU15">
+        <v>0.815</v>
+      </c>
       <c r="AV15"/>
-      <c r="AW15"/>
-      <c r="AX15"/>
-      <c r="AY15"/>
-      <c r="AZ15"/>
-      <c r="BA15"/>
+      <c r="AW15">
+        <v>0.8138348740835193</v>
+      </c>
+      <c r="AX15">
+        <v>0.826171875</v>
+      </c>
+      <c r="AY15">
+        <v>0.8125</v>
+      </c>
+      <c r="AZ15">
+        <v>0.8104838709677419</v>
+      </c>
+      <c r="BA15">
+        <v>0.803921568627451</v>
+      </c>
     </row>
     <row r="16" spans="1:53">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D16">
         <v>0.6362766974816704</v>
@@ -1826,40 +2290,84 @@
       <c r="AA16">
         <v>0.6507692307692308</v>
       </c>
-      <c r="AB16"/>
-      <c r="AC16"/>
+      <c r="AB16">
+        <v>0.6289034132171387</v>
+      </c>
+      <c r="AC16">
+        <v>0.6434955312810328</v>
+      </c>
       <c r="AD16"/>
-      <c r="AE16"/>
-      <c r="AF16"/>
-      <c r="AG16"/>
-      <c r="AH16"/>
-      <c r="AI16"/>
+      <c r="AE16">
+        <v>0.6362766974816704</v>
+      </c>
+      <c r="AF16">
+        <v>0.5584415584415584</v>
+      </c>
+      <c r="AG16">
+        <v>0.6303901437371663</v>
+      </c>
+      <c r="AH16">
+        <v>0.6493699036323203</v>
+      </c>
+      <c r="AI16">
+        <v>0.6363636363636364</v>
+      </c>
       <c r="AJ16"/>
-      <c r="AK16"/>
-      <c r="AL16"/>
-      <c r="AM16"/>
-      <c r="AN16"/>
-      <c r="AO16"/>
+      <c r="AK16">
+        <v>0.6362766974816704</v>
+      </c>
+      <c r="AL16">
+        <v>0.5865384615384616</v>
+      </c>
+      <c r="AM16">
+        <v>0.6011730205278593</v>
+      </c>
+      <c r="AN16">
+        <v>0.6601123595505618</v>
+      </c>
+      <c r="AO16">
+        <v>0.6484641638225256</v>
+      </c>
       <c r="AP16"/>
-      <c r="AQ16"/>
-      <c r="AR16"/>
-      <c r="AS16"/>
-      <c r="AT16"/>
-      <c r="AU16"/>
+      <c r="AQ16">
+        <v>0.6362766974816704</v>
+      </c>
+      <c r="AR16">
+        <v>0.6267409470752089</v>
+      </c>
+      <c r="AS16">
+        <v>0.638854296388543</v>
+      </c>
+      <c r="AT16">
+        <v>0.6481481481481481</v>
+      </c>
+      <c r="AU16">
+        <v>0.575</v>
+      </c>
       <c r="AV16"/>
-      <c r="AW16"/>
-      <c r="AX16"/>
-      <c r="AY16"/>
-      <c r="AZ16"/>
-      <c r="BA16"/>
+      <c r="AW16">
+        <v>0.6362766974816704</v>
+      </c>
+      <c r="AX16">
+        <v>0.634765625</v>
+      </c>
+      <c r="AY16">
+        <v>0.6412037037037037</v>
+      </c>
+      <c r="AZ16">
+        <v>0.6344086021505376</v>
+      </c>
+      <c r="BA16">
+        <v>0.5947712418300654</v>
+      </c>
     </row>
     <row r="17" spans="1:53">
       <c r="A17"/>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D17">
         <v>0.3704175964297099</v>
@@ -1925,40 +2433,84 @@
       <c r="AA17">
         <v>0.33692307692307694</v>
       </c>
-      <c r="AB17"/>
-      <c r="AC17"/>
+      <c r="AB17">
+        <v>0.37254901960784315</v>
+      </c>
+      <c r="AC17">
+        <v>0.38828202581926513</v>
+      </c>
       <c r="AD17"/>
-      <c r="AE17"/>
-      <c r="AF17"/>
-      <c r="AG17"/>
-      <c r="AH17"/>
-      <c r="AI17"/>
+      <c r="AE17">
+        <v>0.3704175964297099</v>
+      </c>
+      <c r="AF17">
+        <v>0.4090909090909091</v>
+      </c>
+      <c r="AG17">
+        <v>0.3490759753593429</v>
+      </c>
+      <c r="AH17">
+        <v>0.374351371386212</v>
+      </c>
+      <c r="AI17">
+        <v>0.38484848484848483</v>
+      </c>
       <c r="AJ17"/>
-      <c r="AK17"/>
-      <c r="AL17"/>
-      <c r="AM17"/>
-      <c r="AN17"/>
-      <c r="AO17"/>
+      <c r="AK17">
+        <v>0.3704175964297099</v>
+      </c>
+      <c r="AL17">
+        <v>0.3942307692307692</v>
+      </c>
+      <c r="AM17">
+        <v>0.36950146627565983</v>
+      </c>
+      <c r="AN17">
+        <v>0.36235955056179775</v>
+      </c>
+      <c r="AO17">
+        <v>0.3873720136518771</v>
+      </c>
       <c r="AP17"/>
-      <c r="AQ17"/>
-      <c r="AR17"/>
-      <c r="AS17"/>
-      <c r="AT17"/>
-      <c r="AU17"/>
+      <c r="AQ17">
+        <v>0.3704175964297099</v>
+      </c>
+      <c r="AR17">
+        <v>0.3788300835654596</v>
+      </c>
+      <c r="AS17">
+        <v>0.35678704856787047</v>
+      </c>
+      <c r="AT17">
+        <v>0.38580246913580246</v>
+      </c>
+      <c r="AU17">
+        <v>0.39</v>
+      </c>
       <c r="AV17"/>
-      <c r="AW17"/>
-      <c r="AX17"/>
-      <c r="AY17"/>
-      <c r="AZ17"/>
-      <c r="BA17"/>
+      <c r="AW17">
+        <v>0.3704175964297099</v>
+      </c>
+      <c r="AX17">
+        <v>0.373046875</v>
+      </c>
+      <c r="AY17">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="AZ17">
+        <v>0.3844086021505376</v>
+      </c>
+      <c r="BA17">
+        <v>0.3202614379084967</v>
+      </c>
     </row>
     <row r="18" spans="1:53">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>0.2843481032833918</v>
@@ -2024,40 +2576,84 @@
       <c r="AA18">
         <v>0.26615384615384613</v>
       </c>
-      <c r="AB18"/>
-      <c r="AC18"/>
+      <c r="AB18">
+        <v>0.29121278140885987</v>
+      </c>
+      <c r="AC18">
+        <v>0.28500496524329694</v>
+      </c>
       <c r="AD18"/>
-      <c r="AE18"/>
-      <c r="AF18"/>
-      <c r="AG18"/>
-      <c r="AH18"/>
-      <c r="AI18"/>
+      <c r="AE18">
+        <v>0.2843481032833918</v>
+      </c>
+      <c r="AF18">
+        <v>0.2987012987012987</v>
+      </c>
+      <c r="AG18">
+        <v>0.2669404517453799</v>
+      </c>
+      <c r="AH18">
+        <v>0.29132690882134915</v>
+      </c>
+      <c r="AI18">
+        <v>0.2924242424242424</v>
+      </c>
       <c r="AJ18"/>
-      <c r="AK18"/>
-      <c r="AL18"/>
-      <c r="AM18"/>
-      <c r="AN18"/>
-      <c r="AO18"/>
+      <c r="AK18">
+        <v>0.2843481032833918</v>
+      </c>
+      <c r="AL18">
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="AM18">
+        <v>0.27663734115347016</v>
+      </c>
+      <c r="AN18">
+        <v>0.28441011235955055</v>
+      </c>
+      <c r="AO18">
+        <v>0.30716723549488056</v>
+      </c>
       <c r="AP18"/>
-      <c r="AQ18"/>
-      <c r="AR18"/>
-      <c r="AS18"/>
-      <c r="AT18"/>
-      <c r="AU18"/>
+      <c r="AQ18">
+        <v>0.2843481032833918</v>
+      </c>
+      <c r="AR18">
+        <v>0.2785515320334262</v>
+      </c>
+      <c r="AS18">
+        <v>0.28393524283935245</v>
+      </c>
+      <c r="AT18">
+        <v>0.28703703703703703</v>
+      </c>
+      <c r="AU18">
+        <v>0.285</v>
+      </c>
       <c r="AV18"/>
-      <c r="AW18"/>
-      <c r="AX18"/>
-      <c r="AY18"/>
-      <c r="AZ18"/>
-      <c r="BA18"/>
+      <c r="AW18">
+        <v>0.2843481032833918</v>
+      </c>
+      <c r="AX18">
+        <v>0.263671875</v>
+      </c>
+      <c r="AY18">
+        <v>0.30324074074074076</v>
+      </c>
+      <c r="AZ18">
+        <v>0.25806451612903225</v>
+      </c>
+      <c r="BA18">
+        <v>0.2679738562091503</v>
+      </c>
     </row>
     <row r="19" spans="1:53">
       <c r="A19"/>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>0.7593241950908511</v>
@@ -2123,40 +2719,84 @@
       <c r="AA19">
         <v>0.7876923076923077</v>
       </c>
-      <c r="AB19"/>
-      <c r="AC19"/>
+      <c r="AB19">
+        <v>0.7458242556281772</v>
+      </c>
+      <c r="AC19">
+        <v>0.7576961271102284</v>
+      </c>
       <c r="AD19"/>
-      <c r="AE19"/>
-      <c r="AF19"/>
-      <c r="AG19"/>
-      <c r="AH19"/>
-      <c r="AI19"/>
+      <c r="AE19">
+        <v>0.7593241950908511</v>
+      </c>
+      <c r="AF19">
+        <v>0.7337662337662337</v>
+      </c>
+      <c r="AG19">
+        <v>0.7351129363449692</v>
+      </c>
+      <c r="AH19">
+        <v>0.7679762787249814</v>
+      </c>
+      <c r="AI19">
+        <v>0.7833333333333333</v>
+      </c>
       <c r="AJ19"/>
-      <c r="AK19"/>
-      <c r="AL19"/>
-      <c r="AM19"/>
-      <c r="AN19"/>
-      <c r="AO19"/>
+      <c r="AK19">
+        <v>0.7593241950908511</v>
+      </c>
+      <c r="AL19">
+        <v>0.7307692307692307</v>
+      </c>
+      <c r="AM19">
+        <v>0.729227761485826</v>
+      </c>
+      <c r="AN19">
+        <v>0.7710674157303371</v>
+      </c>
+      <c r="AO19">
+        <v>0.78839590443686</v>
+      </c>
       <c r="AP19"/>
-      <c r="AQ19"/>
-      <c r="AR19"/>
-      <c r="AS19"/>
-      <c r="AT19"/>
-      <c r="AU19"/>
+      <c r="AQ19">
+        <v>0.7593241950908511</v>
+      </c>
+      <c r="AR19">
+        <v>0.7325905292479109</v>
+      </c>
+      <c r="AS19">
+        <v>0.7615193026151931</v>
+      </c>
+      <c r="AT19">
+        <v>0.7664609053497943</v>
+      </c>
+      <c r="AU19">
+        <v>0.755</v>
+      </c>
       <c r="AV19"/>
-      <c r="AW19"/>
-      <c r="AX19"/>
-      <c r="AY19"/>
-      <c r="AZ19"/>
-      <c r="BA19"/>
+      <c r="AW19">
+        <v>0.7593241950908511</v>
+      </c>
+      <c r="AX19">
+        <v>0.763671875</v>
+      </c>
+      <c r="AY19">
+        <v>0.7604166666666666</v>
+      </c>
+      <c r="AZ19">
+        <v>0.7486559139784946</v>
+      </c>
+      <c r="BA19">
+        <v>0.7843137254901961</v>
+      </c>
     </row>
     <row r="20" spans="1:53">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D20">
         <v>0.4430985017532674</v>
@@ -2222,40 +2862,84 @@
       <c r="AA20">
         <v>0.4323076923076923</v>
       </c>
-      <c r="AB20"/>
-      <c r="AC20"/>
+      <c r="AB20">
+        <v>0.439360929557008</v>
+      </c>
+      <c r="AC20">
+        <v>0.44985104270109233</v>
+      </c>
       <c r="AD20"/>
-      <c r="AE20"/>
-      <c r="AF20"/>
-      <c r="AG20"/>
-      <c r="AH20"/>
-      <c r="AI20"/>
+      <c r="AE20">
+        <v>0.4430985017532674</v>
+      </c>
+      <c r="AF20">
+        <v>0.37012987012987014</v>
+      </c>
+      <c r="AG20">
+        <v>0.4271047227926078</v>
+      </c>
+      <c r="AH20">
+        <v>0.4425500370644922</v>
+      </c>
+      <c r="AI20">
+        <v>0.48484848484848486</v>
+      </c>
       <c r="AJ20"/>
-      <c r="AK20"/>
-      <c r="AL20"/>
-      <c r="AM20"/>
-      <c r="AN20"/>
-      <c r="AO20"/>
+      <c r="AK20">
+        <v>0.4430985017532674</v>
+      </c>
+      <c r="AL20">
+        <v>0.36538461538461536</v>
+      </c>
+      <c r="AM20">
+        <v>0.41055718475073316</v>
+      </c>
+      <c r="AN20">
+        <v>0.45997191011235955</v>
+      </c>
+      <c r="AO20">
+        <v>0.4726962457337884</v>
+      </c>
       <c r="AP20"/>
-      <c r="AQ20"/>
-      <c r="AR20"/>
-      <c r="AS20"/>
-      <c r="AT20"/>
-      <c r="AU20"/>
+      <c r="AQ20">
+        <v>0.4430985017532674</v>
+      </c>
+      <c r="AR20">
+        <v>0.42896935933147634</v>
+      </c>
+      <c r="AS20">
+        <v>0.43711083437110837</v>
+      </c>
+      <c r="AT20">
+        <v>0.44753086419753085</v>
+      </c>
+      <c r="AU20">
+        <v>0.495</v>
+      </c>
       <c r="AV20"/>
-      <c r="AW20"/>
-      <c r="AX20"/>
-      <c r="AY20"/>
-      <c r="AZ20"/>
-      <c r="BA20"/>
+      <c r="AW20">
+        <v>0.4430985017532674</v>
+      </c>
+      <c r="AX20">
+        <v>0.453125</v>
+      </c>
+      <c r="AY20">
+        <v>0.44560185185185186</v>
+      </c>
+      <c r="AZ20">
+        <v>0.4260752688172043</v>
+      </c>
+      <c r="BA20">
+        <v>0.46405228758169936</v>
+      </c>
     </row>
     <row r="21" spans="1:53">
       <c r="A21"/>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D21">
         <v>0.14026139623844439</v>
@@ -2321,40 +3005,84 @@
       <c r="AA21">
         <v>0.12</v>
       </c>
-      <c r="AB21"/>
-      <c r="AC21"/>
+      <c r="AB21">
+        <v>0.13870733478576616</v>
+      </c>
+      <c r="AC21">
+        <v>0.1529294935451837</v>
+      </c>
       <c r="AD21"/>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AG21"/>
-      <c r="AH21"/>
-      <c r="AI21"/>
+      <c r="AE21">
+        <v>0.14026139623844439</v>
+      </c>
+      <c r="AF21">
+        <v>0.12337662337662338</v>
+      </c>
+      <c r="AG21">
+        <v>0.12833675564681724</v>
+      </c>
+      <c r="AH21">
+        <v>0.13936249073387694</v>
+      </c>
+      <c r="AI21">
+        <v>0.16363636363636364</v>
+      </c>
       <c r="AJ21"/>
-      <c r="AK21"/>
-      <c r="AL21"/>
-      <c r="AM21"/>
-      <c r="AN21"/>
-      <c r="AO21"/>
+      <c r="AK21">
+        <v>0.14026139623844439</v>
+      </c>
+      <c r="AL21">
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="AM21">
+        <v>0.13978494623655913</v>
+      </c>
+      <c r="AN21">
+        <v>0.1306179775280899</v>
+      </c>
+      <c r="AO21">
+        <v>0.1621160409556314</v>
+      </c>
       <c r="AP21"/>
-      <c r="AQ21"/>
-      <c r="AR21"/>
-      <c r="AS21"/>
-      <c r="AT21"/>
-      <c r="AU21"/>
+      <c r="AQ21">
+        <v>0.14026139623844439</v>
+      </c>
+      <c r="AR21">
+        <v>0.13649025069637882</v>
+      </c>
+      <c r="AS21">
+        <v>0.13138231631382316</v>
+      </c>
+      <c r="AT21">
+        <v>0.15020576131687244</v>
+      </c>
+      <c r="AU21">
+        <v>0.17</v>
+      </c>
       <c r="AV21"/>
-      <c r="AW21"/>
-      <c r="AX21"/>
-      <c r="AY21"/>
-      <c r="AZ21"/>
-      <c r="BA21"/>
+      <c r="AW21">
+        <v>0.14026139623844439</v>
+      </c>
+      <c r="AX21">
+        <v>0.1640625</v>
+      </c>
+      <c r="AY21">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="AZ21">
+        <v>0.1303763440860215</v>
+      </c>
+      <c r="BA21">
+        <v>0.16339869281045752</v>
+      </c>
     </row>
     <row r="22" spans="1:53">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D22">
         <v>0.000318775900541919</v>
@@ -2403,33 +3131,49 @@
       <c r="AB22"/>
       <c r="AC22"/>
       <c r="AD22"/>
-      <c r="AE22"/>
+      <c r="AE22">
+        <v>0.000318775900541919</v>
+      </c>
       <c r="AF22"/>
-      <c r="AG22"/>
+      <c r="AG22">
+        <v>0.001026694045174538</v>
+      </c>
       <c r="AH22"/>
       <c r="AI22"/>
       <c r="AJ22"/>
-      <c r="AK22"/>
+      <c r="AK22">
+        <v>0.000318775900541919</v>
+      </c>
       <c r="AL22"/>
       <c r="AM22"/>
-      <c r="AN22"/>
+      <c r="AN22">
+        <v>0.0007022471910112359</v>
+      </c>
       <c r="AO22"/>
       <c r="AP22"/>
-      <c r="AQ22"/>
+      <c r="AQ22">
+        <v>0.000318775900541919</v>
+      </c>
       <c r="AR22"/>
-      <c r="AS22"/>
+      <c r="AS22">
+        <v>0.0006226650062266501</v>
+      </c>
       <c r="AT22"/>
       <c r="AU22"/>
       <c r="AV22"/>
-      <c r="AW22"/>
+      <c r="AW22">
+        <v>0.000318775900541919</v>
+      </c>
       <c r="AX22"/>
       <c r="AY22"/>
-      <c r="AZ22"/>
+      <c r="AZ22">
+        <v>0.0013440860215053765</v>
+      </c>
       <c r="BA22"/>
     </row>
     <row r="23" spans="1:53">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>

</xml_diff>